<commit_message>
feat(tsmaster) : update version to 5.0
Description:
    - 适配了同星的CAN盒
    - 修改了类型提示
    - 修复了android service的问题
    - 完成了测试用例生成器（简版）
    - 调整了代码结构

Change-Id: I15218d249fa649dff1fbf52c9dac19922e150a05
</commit_message>
<xml_diff>
--- a/src/automotive/application/testcase/writer/template.xlsx
+++ b/src/automotive/application/testcase/writer/template.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Temporary\python-automotive\src\automotive\application\testcase\writer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\chinatsp\develop\python\src\automotive\application\testcase\writer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5B074CF-F483-4F8D-9E4F-FA13CDD02DEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13650" yWindow="7845" windowWidth="13905" windowHeight="14070" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13650" yWindow="7845" windowWidth="13905" windowHeight="14070" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -135,7 +134,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -332,6 +331,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -366,9 +368,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -650,7 +649,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -660,23 +659,23 @@
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
-      <c r="N1" s="8"/>
-      <c r="O1" s="9"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
+      <c r="O1" s="10"/>
     </row>
     <row r="2" spans="1:15" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -685,22 +684,22 @@
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="11"/>
-      <c r="E2" s="12" t="s">
+      <c r="D2" s="12"/>
+      <c r="E2" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="13"/>
-      <c r="G2" s="14" t="s">
+      <c r="F2" s="14"/>
+      <c r="G2" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="15"/>
-      <c r="I2" s="16" t="s">
+      <c r="H2" s="16"/>
+      <c r="I2" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="17"/>
+      <c r="J2" s="18"/>
       <c r="K2" s="2" t="s">
         <v>7</v>
       </c>
@@ -732,11 +731,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:O3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -749,25 +748,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="15" x14ac:dyDescent="0.2">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18" t="s">
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
-      <c r="N1" s="18"/>
-      <c r="O1" s="18"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19"/>
+      <c r="N1" s="19"/>
+      <c r="O1" s="19"/>
     </row>
     <row r="2" spans="1:15" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
@@ -791,7 +790,7 @@
       <c r="G2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="19" t="s">
+      <c r="H2" s="7" t="s">
         <v>27</v>
       </c>
       <c r="I2" s="5" t="s">
@@ -815,9 +814,6 @@
       <c r="O2" s="5" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" ht="15" x14ac:dyDescent="0.2">
-      <c r="O3" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
feat(result) : add result in writer and reader
Description:
   增加了xmind添加测试结果的功能

Change-Id: Ifab63689c644bf8e95e0f64f04eb1cf107ae753c
</commit_message>
<xml_diff>
--- a/src/automotive/application/testcase/writer/template.xlsx
+++ b/src/automotive/application/testcase/writer/template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\chinatsp\develop\python\src\automotive\application\testcase\writer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\Chinatsp\release\python\src\automotive\application\testcase\writer\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -66,9 +66,6 @@
     <t>用例信息</t>
   </si>
   <si>
-    <t>第六轮测试结果</t>
-  </si>
-  <si>
     <t>用例名称</t>
   </si>
   <si>
@@ -128,6 +125,10 @@
       </rPr>
       <t>ID</t>
     </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>测试结果</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -309,7 +310,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -368,6 +369,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -735,7 +739,7 @@
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -760,8 +764,8 @@
       <c r="H1" s="19"/>
       <c r="I1" s="19"/>
       <c r="J1" s="19"/>
-      <c r="K1" s="19" t="s">
-        <v>13</v>
+      <c r="K1" s="20" t="s">
+        <v>27</v>
       </c>
       <c r="L1" s="19"/>
       <c r="M1" s="19"/>
@@ -773,46 +777,46 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" s="5" t="s">
+      <c r="I2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="I2" s="5" t="s">
+      <c r="J2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="K2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="L2" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="M2" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="N2" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="N2" s="5" t="s">
+      <c r="O2" s="5" t="s">
         <v>24</v>
-      </c>
-      <c r="O2" s="5" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix(testcase) : fix testcase generator some issue
Description:
   修复了测试用例生成器的问题

Change-Id: I7bdc4c1e260fd6c5c0d59a10330d548299527701
</commit_message>
<xml_diff>
--- a/src/automotive/application/testcase/writer/template.xlsx
+++ b/src/automotive/application/testcase/writer/template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\Chinatsp\release\python\src\automotive\application\testcase\writer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\chinatsp\develop\python\src\automotive\application\testcase\writer\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -66,6 +66,9 @@
     <t>用例信息</t>
   </si>
   <si>
+    <t>第六轮测试结果</t>
+  </si>
+  <si>
     <t>用例名称</t>
   </si>
   <si>
@@ -125,10 +128,6 @@
       </rPr>
       <t>ID</t>
     </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>测试结果</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -310,7 +309,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -369,9 +368,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -739,7 +735,7 @@
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -764,8 +760,8 @@
       <c r="H1" s="19"/>
       <c r="I1" s="19"/>
       <c r="J1" s="19"/>
-      <c r="K1" s="20" t="s">
-        <v>27</v>
+      <c r="K1" s="19" t="s">
+        <v>13</v>
       </c>
       <c r="L1" s="19"/>
       <c r="M1" s="19"/>
@@ -777,46 +773,46 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="O2" s="5" t="s">
         <v>25</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="M2" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="N2" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="O2" s="5" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>